<commit_message>
something in the scedhule
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
   <si>
     <t>פרק</t>
   </si>
@@ -133,22 +133,28 @@
 https://towardsdatascience.com/https-medium-com-talperetz24-mastering-the-new-generation-of-gradient-boosting-db04062a7ea2</t>
   </si>
   <si>
-    <t>במאמר: לפרט פרקים רלוונטים לא (למשל: ניסויים פחות מעניין). 
+    <t>נספחים</t>
+  </si>
+  <si>
+    <t>סקר ספרות</t>
+  </si>
+  <si>
+    <t>לקרוא, לחקור, לסכם, להשוות, לשאול שאלות, למצוא תשובות על Bayesian hyper parameter optimization</t>
+  </si>
+  <si>
+    <t>אולי צריך להוסיף דוגמה של סקירה כדי לדעת מה הרמה הנדרשת (אורך, פורמט וכו')</t>
+  </si>
+  <si>
+    <t>Kaggle</t>
+  </si>
+  <si>
+    <t>עבודה עם הדאטה של NYC taxi fare prediction</t>
+  </si>
+  <si>
+    <t>במאמר: לפרט פרקים רלוונטים ולא רלוונטים (למשל: ניסויים פחות מעניין). 
 בלוגפוסטים קשוחים (LIGHTGBM, CATBOOST).
 בלוגפוסט על CATBOOST שעוזר להבין את הרעיון של Ordered Boosting: http://towardsdatascience.com/catboost-d1f1366aca34
 יש סדרת סרטונים ביוטיוב (סה"כ ~100 דקות) של statquest שמסבירים XGBOOST בצורה מאד פשוטה</t>
-  </si>
-  <si>
-    <t>נספחים</t>
-  </si>
-  <si>
-    <t>סקר ספרות</t>
-  </si>
-  <si>
-    <t>לקרוא, לחקור, לסכם, להשוות, לשאול שאלות, למצוא תשובות על Bayesian hyper parameter optimization</t>
-  </si>
-  <si>
-    <t>אולי צריך להוסיף דוגמה של סקירה כדי לדעת מה הרמה הנדרשת (אורך, פורמט וכו')</t>
   </si>
 </sst>
 </file>
@@ -156,7 +162,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -201,7 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -212,10 +218,10 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -537,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -934,36 +940,53 @@
         <v>1</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
         <v>37</v>
       </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="E17" s="2">
         <v>43985.418055555558</v>
       </c>
       <c r="F17" s="2">
-        <v>43985.710416666669</v>
+        <v>43986.793055555558</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
         <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="2">
+        <v>43986.59097222222</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Chapter 6 - SVM and Bayesian learning
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
   <si>
     <t>פרק</t>
   </si>
@@ -192,6 +192,24 @@
   </si>
   <si>
     <t>בוצע במקום kaggle שהדאטה שלו לא זמין</t>
+  </si>
+  <si>
+    <t>ISLR 337-359
+שאלות 3,6 ועוד כמה מההוראות בדרייב</t>
+  </si>
+  <si>
+    <t>תרגיל 6 ב ISLR מרגיש מיותר ומנסה להעביר נקודה שדי פשוט להבין מהקריאה עצמה
+ב Part 4 ב drive יוצא (לי, אולי אני בעייתי) ששני המודלים מסווגים הכל כ-0 בגלל שהדאטה לא מאוזן.</t>
+  </si>
+  <si>
+    <t>deep learning 5.6
+Bishop 3.3-3.3.1
+חלק כלשהו מהקורס ב MIT
+Intoduction to Probability 8</t>
+  </si>
+  <si>
+    <t>עדיף להתחיל מקריאה של הבלוג פוסטים לפני שנכנסים לקריאה בספרים (שרובה הרגישה לא הכי חיונית). 
+אם אפשר כדאי (לדעתי) להוסיף תרגיל לפרק (גם אם משהו קטן של שימוש ב PYMC3)</t>
   </si>
 </sst>
 </file>
@@ -578,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,6 +1170,12 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
       <c r="C23" t="s">
         <v>16</v>
       </c>
@@ -1161,32 +1185,99 @@
       <c r="E23" s="2">
         <v>43999.332638888889</v>
       </c>
+      <c r="F23" s="2">
+        <v>43999.537499999999</v>
+      </c>
+      <c r="G23">
+        <v>0.5</v>
+      </c>
+      <c r="H23">
+        <v>0.5</v>
+      </c>
       <c r="I23" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="2">
+        <v>43999.59097222222</v>
+      </c>
+      <c r="F24" s="2">
+        <v>44000.605555555558</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0.75</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="2">
+        <v>44000.615972222222</v>
+      </c>
+      <c r="F25" s="2">
+        <v>44004.611111111109</v>
+      </c>
+      <c r="G25">
+        <v>2.25</v>
+      </c>
+      <c r="H25">
+        <v>1.75</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Clustering - kind of theoretical part
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
   <si>
     <t>פרק</t>
   </si>
@@ -210,6 +210,22 @@
   <si>
     <t>עדיף להתחיל מקריאה של הבלוג פוסטים לפני שנכנסים לקריאה בספרים (שרובה הרגישה לא הכי חיונית). 
 אם אפשר כדאי (לדעתי) להוסיף תרגיל לפרק (גם אם משהו קטן של שימוש ב PYMC3)</t>
+  </si>
+  <si>
+    <t>קריאה+תרגיל</t>
+  </si>
+  <si>
+    <t>Data Mining 443-469
+Data Mining 483-491
+Star image exercise
+Another exercise (P-DBSCAN)</t>
+  </si>
+  <si>
+    <t>הכותרות לא מתאימות לתתי הפרקים (בפרק של DBSCAN קוראים על כמה שיטות Density based וכו')
+חסר קובץ Data.csv
+במאמר מוצג אלגוריתם 1 (ולא שניים כמו שכתוב בהוראות), ונראה שהוא לא מתאים לדאטה שתואר בתרגיל (המאמר מניח שיש מידע בסגנון של "owner" בנוסף לפיצ'רים הרגילים)
+(דילגתי על החלק הזה של התרגיל בגלל הנ"ל)
+יכול להיות רעיון נחמד לתת לממש איזה אלגוריתם או שניים tough</t>
   </si>
 </sst>
 </file>
@@ -598,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,14 +1272,33 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>6</v>
+    <row r="26" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="2">
+        <v>44005.381944444445</v>
+      </c>
+      <c r="F26" s="2">
+        <v>44007.446527777778</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
semi supervised literature survey
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="64">
   <si>
     <t>פרק</t>
   </si>
@@ -236,6 +236,13 @@
   </si>
   <si>
     <t>לקרוא, לחקור, לסכם, להשוות, לשאול שאלות, למצוא תשובות על semi supervised learning</t>
+  </si>
+  <si>
+    <t>6/30/2020 6/29/20 10:21</t>
+  </si>
+  <si>
+    <t>בלוגפוסט שווה אחוששלוקי https://ruder.io/semi-supervised/
+לדעתי, הנושא הזה צריך לבוא אחרי הפרק של רשתות כי יש שיטות שרלוונטיות בעיקר לזה. בכלל, הנושא הזה יותר מתאים לתמונות.</t>
   </si>
 </sst>
 </file>
@@ -637,7 +644,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1352,7 +1359,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -1364,6 +1371,21 @@
       </c>
       <c r="D28" s="1" t="s">
         <v>61</v>
+      </c>
+      <c r="E28" s="2">
+        <v>44011.447916666664</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Literature survey - unbalanced dataset
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="91">
   <si>
     <t>פרק</t>
   </si>
@@ -331,7 +331,21 @@
   </si>
   <si>
     <t>הייתי צריך 3 ימים כדי להבין שהדאטה הוא כמה קטעי סיגנלים שחתכו לחלקים בגודל 128
-LSTM לא עובד לי כל כך והרבה זמן (~1.5 ימים נטו הלכו לי על לנסות לתפעל את זה)</t>
+LSTM לא עובד לי כל כך והרבה זמן (~1.5 ימים נטו הלכו לי על לנסות לתפעל את זה)
+ב-30.7 עשיתי הפסקה מתודית בשביל סקירות ספרות</t>
+  </si>
+  <si>
+    <t>חפיפה גדולה עם הפרק על עצים</t>
+  </si>
+  <si>
+    <t>לקרוא, לחקור, לסכם, להשוות, לשאול שאלות, למצוא תשובות על ensemble learning</t>
+  </si>
+  <si>
+    <t>לקרוא, לחקור, לסכם, להשוות, לשאול שאלות, למצוא תשובות על unbalanced dataset</t>
+  </si>
+  <si>
+    <t>לכוון לנושאים יותר ספציפיים כי תמיד מגיעים לאותן 2.5 שיטות לטיפול בבעיה.
+רלוונטי לכל הסקירות: להוסיף אותן במקומות ספציפייים בהכשרה (בשלב הזה זה מרגיש מאוחר מדי)</t>
   </si>
 </sst>
 </file>
@@ -730,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D36" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1738,7 +1752,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>9</v>
       </c>
@@ -1756,6 +1770,64 @@
       </c>
       <c r="I38" s="1" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E39" s="2">
+        <v>44042.367361111108</v>
+      </c>
+      <c r="F39" s="2">
+        <v>44042.462500000001</v>
+      </c>
+      <c r="G39">
+        <v>0.25</v>
+      </c>
+      <c r="H39">
+        <v>0.25</v>
+      </c>
+      <c r="I39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E40" s="2">
+        <v>44042.502083333333</v>
+      </c>
+      <c r="F40" s="2">
+        <v>44042.64166666667</v>
+      </c>
+      <c r="G40">
+        <v>0.5</v>
+      </c>
+      <c r="H40">
+        <v>0.25</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Literature survey - feature selection and stuff
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="6970"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="6380"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="94">
   <si>
     <t>פרק</t>
   </si>
@@ -346,6 +346,16 @@
   <si>
     <t>לכוון לנושאים יותר ספציפיים כי תמיד מגיעים לאותן 2.5 שיטות לטיפול בבעיה.
 רלוונטי לכל הסקירות: להוסיף אותן במקומות ספציפייים בהכשרה (בשלב הזה זה מרגיש מאוחר מדי)</t>
+  </si>
+  <si>
+    <t>נושא יחסית גנרי (או שלא הבנתי טוב)
+פוסט נחמד בנושא https://www.kaggle.com/residentmario/automated-feature-selection-with-sklearn</t>
+  </si>
+  <si>
+    <t>7/30/2020 16:00 PM</t>
+  </si>
+  <si>
+    <t>לקרוא, לחקור, לסכם, להשוות, לשאול שאלות, למצוא תשובות על בחירת פיצ'רים</t>
   </si>
 </sst>
 </file>
@@ -744,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1830,6 +1840,35 @@
         <v>90</v>
       </c>
     </row>
+    <row r="41" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41" s="2">
+        <v>44042.816666666666</v>
+      </c>
+      <c r="G41">
+        <v>0.5</v>
+      </c>
+      <c r="H41">
+        <v>0.5</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D14" r:id="rId1" display="https://quantdare.com/isolation-forest-algorithm/_x000a_"/>

</xml_diff>

<commit_message>
updated auto feature ENGENEERING
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -348,14 +348,15 @@
 רלוונטי לכל הסקירות: להוסיף אותן במקומות ספציפייים בהכשרה (בשלב הזה זה מרגיש מאוחר מדי)</t>
   </si>
   <si>
+    <t>7/30/2020 16:00 PM</t>
+  </si>
+  <si>
+    <t>לקרוא, לחקור, לסכם, להשוות, לשאול שאלות, למצוא תשובות על בחירת פיצ'רים</t>
+  </si>
+  <si>
     <t>נושא יחסית גנרי (או שלא הבנתי טוב)
-פוסט נחמד בנושא https://www.kaggle.com/residentmario/automated-feature-selection-with-sklearn</t>
-  </si>
-  <si>
-    <t>7/30/2020 16:00 PM</t>
-  </si>
-  <si>
-    <t>לקרוא, לחקור, לסכם, להשוות, לשאול שאלות, למצוא תשובות על בחירת פיצ'רים</t>
+פוסט נחמד בנושא https://www.kaggle.com/residentmario/automated-feature-selection-with-sklearn
+הסבר טוב על featuretools https://towardsdatascience.com/automated-feature-engineering-in-python-99baf11cc219</t>
   </si>
 </sst>
 </file>
@@ -756,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D38" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1840,7 +1841,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>37</v>
       </c>
@@ -1851,22 +1852,22 @@
         <v>38</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F41" s="2">
+        <v>44045.739583333336</v>
+      </c>
+      <c r="G41">
+        <v>1.5</v>
+      </c>
+      <c r="H41">
+        <v>0.75</v>
+      </c>
+      <c r="I41" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F41" s="2">
-        <v>44042.816666666666</v>
-      </c>
-      <c r="G41">
-        <v>0.5</v>
-      </c>
-      <c r="H41">
-        <v>0.5</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatic feature engeneering - TPOT and stuff tryout
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -758,7 +758,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D38" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1864,7 +1864,7 @@
         <v>1.5</v>
       </c>
       <c r="H41">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>93</v>

</xml_diff>